<commit_message>
cambio de tema, reporte
</commit_message>
<xml_diff>
--- a/resources/api/public/files/rptpc.xlsx
+++ b/resources/api/public/files/rptpc.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gsystemperu\kokojump\resources\api\public\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="17595" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17595" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="reporte" sheetId="1" r:id="rId1"/>
+    <sheet name="reporte efectivo" sheetId="1" r:id="rId1"/>
+    <sheet name="reporte tarjeta" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Reporte de Ventas Diarias</t>
   </si>
@@ -40,14 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -68,159 +68,8 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,198 +78,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.25"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -428,253 +91,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -703,59 +124,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
-    <cellStyle name="60% - Accent2" xfId="11" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="12" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="14" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="15" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="16" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="17" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="19" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="20" builtinId="32"/>
-    <cellStyle name="Bad" xfId="21" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="22" builtinId="23"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Moneda" xfId="32" builtinId="4"/>
-    <cellStyle name="Heading 2" xfId="33" builtinId="17"/>
-    <cellStyle name="Heading 1" xfId="34" builtinId="16"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Warning Text" xfId="36" builtinId="11"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Coma[0]" xfId="39" builtinId="6"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8"/>
-    <cellStyle name="Heading 3" xfId="41" builtinId="18"/>
-    <cellStyle name="Moneda[0]" xfId="42" builtinId="7"/>
-    <cellStyle name="20% - Accent4" xfId="43" builtinId="42"/>
-    <cellStyle name="40% - Accent3" xfId="44" builtinId="39"/>
-    <cellStyle name="Linked Cell" xfId="45" builtinId="24"/>
-    <cellStyle name="Accent4" xfId="46" builtinId="41"/>
-    <cellStyle name="Porcentaje" xfId="47" builtinId="5"/>
-    <cellStyle name="Coma" xfId="48" builtinId="3"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -764,7 +155,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="2E3436"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1045,35 +436,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.86" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28666666666667" customWidth="1"/>
-    <col min="2" max="2" width="32.6" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5733333333333" customWidth="1"/>
-    <col min="4" max="4" width="29.7133333333333" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.2866666666667" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.86" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="32.1" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" ht="22" customHeight="1" spans="1:6">
+      <c r="B1" s="11"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="21.95" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1101,17 +491,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
@@ -2452,11 +1842,1155 @@
       <c r="C283" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F283"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32.1" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="7"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="7"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="7"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="7"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="7"/>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="7"/>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="7"/>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="7"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="7"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="7"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="7"/>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="7"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="7"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="7"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="7"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="7"/>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="7"/>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="7"/>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="7"/>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="7"/>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="7"/>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="7"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="7"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="7"/>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="7"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="7"/>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="7"/>
+      <c r="C63" s="7"/>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="7"/>
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="7"/>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="7"/>
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="7"/>
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="7"/>
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="7"/>
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="7"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="7"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="7"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="7"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="7"/>
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="7"/>
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="7"/>
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="7"/>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="7"/>
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="7"/>
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="7"/>
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="7"/>
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="7"/>
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="7"/>
+      <c r="C83" s="7"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="7"/>
+      <c r="C84" s="7"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="7"/>
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="7"/>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="7"/>
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="7"/>
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="7"/>
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="7"/>
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="7"/>
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="7"/>
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="7"/>
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="7"/>
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="7"/>
+      <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="7"/>
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="7"/>
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="7"/>
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="7"/>
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="7"/>
+      <c r="C100" s="7"/>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="7"/>
+      <c r="C101" s="7"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="7"/>
+      <c r="C102" s="7"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="7"/>
+      <c r="C103" s="7"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="7"/>
+      <c r="C104" s="7"/>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="7"/>
+      <c r="C105" s="7"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="7"/>
+      <c r="C106" s="7"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="7"/>
+      <c r="C107" s="7"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="7"/>
+      <c r="C108" s="7"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="7"/>
+      <c r="C109" s="7"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="7"/>
+      <c r="C110" s="7"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="7"/>
+      <c r="C111" s="7"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="7"/>
+      <c r="C112" s="7"/>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="7"/>
+      <c r="C113" s="7"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="7"/>
+      <c r="C114" s="7"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="7"/>
+      <c r="C115" s="7"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="7"/>
+      <c r="C116" s="7"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="7"/>
+      <c r="C117" s="7"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="7"/>
+      <c r="C118" s="7"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="7"/>
+      <c r="C119" s="7"/>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="7"/>
+      <c r="C120" s="7"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="7"/>
+      <c r="C121" s="7"/>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="7"/>
+      <c r="C122" s="7"/>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="7"/>
+      <c r="C123" s="7"/>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="7"/>
+      <c r="C124" s="7"/>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="7"/>
+      <c r="C125" s="7"/>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="7"/>
+      <c r="C126" s="7"/>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="7"/>
+      <c r="C127" s="7"/>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="7"/>
+      <c r="C128" s="7"/>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="7"/>
+      <c r="C129" s="7"/>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="7"/>
+      <c r="C130" s="7"/>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="7"/>
+      <c r="C131" s="7"/>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="7"/>
+      <c r="C132" s="7"/>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="7"/>
+      <c r="C133" s="7"/>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="7"/>
+      <c r="C134" s="7"/>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="7"/>
+      <c r="C135" s="7"/>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="7"/>
+      <c r="C136" s="7"/>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="7"/>
+      <c r="C137" s="7"/>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="7"/>
+      <c r="C138" s="7"/>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="7"/>
+      <c r="C139" s="7"/>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="7"/>
+      <c r="C140" s="7"/>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="7"/>
+      <c r="C141" s="7"/>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="7"/>
+      <c r="C142" s="7"/>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="7"/>
+      <c r="C143" s="7"/>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="7"/>
+      <c r="C144" s="7"/>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="7"/>
+      <c r="C145" s="7"/>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="7"/>
+      <c r="C146" s="7"/>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="7"/>
+      <c r="C147" s="7"/>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="7"/>
+      <c r="C148" s="7"/>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="7"/>
+      <c r="C149" s="7"/>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="7"/>
+      <c r="C150" s="7"/>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="7"/>
+      <c r="C151" s="7"/>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="7"/>
+      <c r="C152" s="7"/>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="7"/>
+      <c r="C153" s="7"/>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="7"/>
+      <c r="C154" s="7"/>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="7"/>
+      <c r="C155" s="7"/>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="7"/>
+      <c r="C156" s="7"/>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="7"/>
+      <c r="C157" s="7"/>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="7"/>
+      <c r="C158" s="7"/>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="7"/>
+      <c r="C159" s="7"/>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="7"/>
+      <c r="C160" s="7"/>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="7"/>
+      <c r="C161" s="7"/>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="7"/>
+      <c r="C162" s="7"/>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="7"/>
+      <c r="C163" s="7"/>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="7"/>
+      <c r="C164" s="7"/>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="7"/>
+      <c r="C165" s="7"/>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="7"/>
+      <c r="C166" s="7"/>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="7"/>
+      <c r="C167" s="7"/>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="7"/>
+      <c r="C168" s="7"/>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="7"/>
+      <c r="C169" s="7"/>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="7"/>
+      <c r="C170" s="7"/>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="7"/>
+      <c r="C171" s="7"/>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="7"/>
+      <c r="C172" s="7"/>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="7"/>
+      <c r="C173" s="7"/>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="7"/>
+      <c r="C174" s="7"/>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="7"/>
+      <c r="C175" s="7"/>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="7"/>
+      <c r="C176" s="7"/>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="7"/>
+      <c r="C177" s="7"/>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="7"/>
+      <c r="C178" s="7"/>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="7"/>
+      <c r="C179" s="7"/>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="7"/>
+      <c r="C180" s="7"/>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="7"/>
+      <c r="C181" s="7"/>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="7"/>
+      <c r="C182" s="7"/>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="7"/>
+      <c r="C183" s="7"/>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="7"/>
+      <c r="C184" s="7"/>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="7"/>
+      <c r="C185" s="7"/>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="7"/>
+      <c r="C186" s="7"/>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="7"/>
+      <c r="C187" s="7"/>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="7"/>
+      <c r="C188" s="7"/>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="7"/>
+      <c r="C189" s="7"/>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="7"/>
+      <c r="C190" s="7"/>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="7"/>
+      <c r="C191" s="7"/>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="7"/>
+      <c r="C192" s="7"/>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="7"/>
+      <c r="C193" s="7"/>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="7"/>
+      <c r="C194" s="7"/>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="7"/>
+      <c r="C195" s="7"/>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="7"/>
+      <c r="C196" s="7"/>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="7"/>
+      <c r="C197" s="7"/>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="7"/>
+      <c r="C198" s="7"/>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="7"/>
+      <c r="C199" s="7"/>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="7"/>
+      <c r="C200" s="7"/>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="7"/>
+      <c r="C201" s="7"/>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="7"/>
+      <c r="C202" s="7"/>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="7"/>
+      <c r="C203" s="7"/>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="7"/>
+      <c r="C204" s="7"/>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="7"/>
+      <c r="C205" s="7"/>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="7"/>
+      <c r="C206" s="7"/>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="7"/>
+      <c r="C207" s="7"/>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="7"/>
+      <c r="C208" s="7"/>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="7"/>
+      <c r="C209" s="7"/>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="7"/>
+      <c r="C210" s="7"/>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="7"/>
+      <c r="C211" s="7"/>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="7"/>
+      <c r="C212" s="7"/>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="7"/>
+      <c r="C213" s="7"/>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="7"/>
+      <c r="C214" s="7"/>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="7"/>
+      <c r="C215" s="7"/>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="7"/>
+      <c r="C216" s="7"/>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="7"/>
+      <c r="C217" s="7"/>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="7"/>
+      <c r="C218" s="7"/>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="7"/>
+      <c r="C219" s="7"/>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="7"/>
+      <c r="C220" s="7"/>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="7"/>
+      <c r="C221" s="7"/>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="7"/>
+      <c r="C222" s="7"/>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="7"/>
+      <c r="C223" s="7"/>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="7"/>
+      <c r="C224" s="7"/>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="7"/>
+      <c r="C225" s="7"/>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="7"/>
+      <c r="C226" s="7"/>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="7"/>
+      <c r="C227" s="7"/>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="7"/>
+      <c r="C228" s="7"/>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="7"/>
+      <c r="C229" s="7"/>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="7"/>
+      <c r="C230" s="7"/>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="7"/>
+      <c r="C231" s="7"/>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="7"/>
+      <c r="C232" s="7"/>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="7"/>
+      <c r="C233" s="7"/>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="7"/>
+      <c r="C234" s="7"/>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="7"/>
+      <c r="C235" s="7"/>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="7"/>
+      <c r="C236" s="7"/>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="7"/>
+      <c r="C237" s="7"/>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="7"/>
+      <c r="C238" s="7"/>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="7"/>
+      <c r="C239" s="7"/>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="7"/>
+      <c r="C240" s="7"/>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="7"/>
+      <c r="C241" s="7"/>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="7"/>
+      <c r="C242" s="7"/>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="7"/>
+      <c r="C243" s="7"/>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="7"/>
+      <c r="C244" s="7"/>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="7"/>
+      <c r="C245" s="7"/>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="7"/>
+      <c r="C246" s="7"/>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="7"/>
+      <c r="C247" s="7"/>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="7"/>
+      <c r="C248" s="7"/>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="7"/>
+      <c r="C249" s="7"/>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="7"/>
+      <c r="C250" s="7"/>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="7"/>
+      <c r="C251" s="7"/>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="7"/>
+      <c r="C252" s="7"/>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="7"/>
+      <c r="C253" s="7"/>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="7"/>
+      <c r="C254" s="7"/>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="7"/>
+      <c r="C255" s="7"/>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="7"/>
+      <c r="C256" s="7"/>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="7"/>
+      <c r="C257" s="7"/>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="7"/>
+      <c r="C258" s="7"/>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="7"/>
+      <c r="C259" s="7"/>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="7"/>
+      <c r="C260" s="7"/>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="7"/>
+      <c r="C261" s="7"/>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="7"/>
+      <c r="C262" s="7"/>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="7"/>
+      <c r="C263" s="7"/>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="7"/>
+      <c r="C264" s="7"/>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="7"/>
+      <c r="C265" s="7"/>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="7"/>
+      <c r="C266" s="7"/>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="7"/>
+      <c r="C267" s="7"/>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="7"/>
+      <c r="C268" s="7"/>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="7"/>
+      <c r="C269" s="7"/>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="7"/>
+      <c r="C270" s="7"/>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="7"/>
+      <c r="C271" s="7"/>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="7"/>
+      <c r="C272" s="7"/>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="7"/>
+      <c r="C273" s="7"/>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="7"/>
+      <c r="C274" s="7"/>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="7"/>
+      <c r="C275" s="7"/>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="7"/>
+      <c r="C276" s="7"/>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="7"/>
+      <c r="C277" s="7"/>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="7"/>
+      <c r="C278" s="7"/>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="7"/>
+      <c r="C279" s="7"/>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="7"/>
+      <c r="C280" s="7"/>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="7"/>
+      <c r="C281" s="7"/>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="7"/>
+      <c r="C282" s="7"/>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="7"/>
+      <c r="C283" s="7"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>